<commit_message>
(#92)added basic clinicsl trials searh form functionality tests
</commit_message>
<xml_diff>
--- a/test-data/cts-data.xlsx
+++ b/test-data/cts-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mashkinaea/IdeaProjects/cgov-digital-platform-qa/test-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C36C604-FAC4-C348-A436-E27A19BCB2CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BEF2557-EC04-FC44-9CBA-151CD1194C2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14540" activeTab="2" xr2:uid="{02E62B52-A561-7E40-BFFB-9E993FCF680A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="36">
   <si>
     <t>path</t>
   </si>
@@ -120,9 +120,6 @@
     <t>CancerKeyWords</t>
   </si>
   <si>
-    <t>breast cancer</t>
-  </si>
-  <si>
     <t>chicken</t>
   </si>
   <si>
@@ -132,46 +129,19 @@
     <t>0000</t>
   </si>
   <si>
-    <t>ZipQuery</t>
-  </si>
-  <si>
-    <t>z</t>
-  </si>
-  <si>
-    <t>AgeQuery</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>t</t>
-  </si>
-  <si>
-    <t>CTQuery</t>
-  </si>
-  <si>
-    <t>KeyWordQuery</t>
-  </si>
-  <si>
-    <t>q</t>
-  </si>
-  <si>
-    <t>ResultsQuery</t>
-  </si>
-  <si>
-    <t>rl</t>
+    <t>ZipCodeInvalid</t>
+  </si>
+  <si>
+    <t>Please enter a valid 5 digit U.S. zip code</t>
+  </si>
+  <si>
+    <t>burkit lymphoma</t>
   </si>
   <si>
     <t>Results</t>
   </si>
   <si>
-    <t>ZipCodeInvalid</t>
-  </si>
-  <si>
-    <t>Please enter a valid 5 digit U.S. zip code</t>
-  </si>
-  <si>
-    <t>burkit lymphoma</t>
+    <t>bilateral cancer</t>
   </si>
 </sst>
 </file>
@@ -594,23 +564,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0BCB40F-6965-4647-B9F4-0250EB72F8C6}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="39.5" customWidth="1"/>
     <col min="2" max="2" width="44.33203125" customWidth="1"/>
-    <col min="3" max="3" width="8" customWidth="1"/>
-    <col min="8" max="9" width="29.6640625" customWidth="1"/>
-    <col min="10" max="10" width="17.33203125" customWidth="1"/>
-    <col min="11" max="11" width="11.83203125" customWidth="1"/>
+    <col min="5" max="5" width="29.6640625" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -618,262 +586,157 @@
         <v>5</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
-        <v>33</v>
+      <c r="C2">
+        <v>90012</v>
       </c>
       <c r="D2">
-        <v>90012</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F2">
-        <v>18</v>
-      </c>
-      <c r="G2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="K2" t="s">
-        <v>30</v>
-      </c>
-      <c r="L2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3">
+        <v>77001</v>
+      </c>
+      <c r="D3">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D3">
-        <v>77001</v>
-      </c>
-      <c r="E3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3">
-        <v>20</v>
-      </c>
-      <c r="G3" t="s">
-        <v>36</v>
-      </c>
-      <c r="H3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" t="s">
-        <v>39</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="K3" t="s">
-        <v>30</v>
-      </c>
-      <c r="L3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
-        <v>33</v>
+      <c r="C4">
+        <v>33101</v>
       </c>
       <c r="D4">
-        <v>33101</v>
+        <v>40</v>
       </c>
       <c r="E4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4">
-        <v>40</v>
-      </c>
-      <c r="G4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H4" t="s">
         <v>23</v>
       </c>
-      <c r="I4" t="s">
-        <v>39</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="K4" t="s">
-        <v>30</v>
-      </c>
-      <c r="L4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
-        <v>33</v>
+      <c r="C5">
+        <v>98105</v>
       </c>
       <c r="D5">
-        <v>98105</v>
+        <v>70</v>
       </c>
       <c r="E5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F5">
-        <v>70</v>
-      </c>
-      <c r="G5" t="s">
-        <v>36</v>
-      </c>
-      <c r="H5" t="s">
         <v>24</v>
       </c>
-      <c r="I5" t="s">
-        <v>39</v>
-      </c>
-      <c r="J5" s="2">
+      <c r="F5" s="2">
         <v>123</v>
       </c>
-      <c r="K5" t="s">
-        <v>30</v>
-      </c>
-      <c r="L5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
       </c>
-      <c r="C6" t="s">
-        <v>33</v>
+      <c r="C6">
+        <v>22030</v>
       </c>
       <c r="D6">
-        <v>22030</v>
+        <v>120</v>
       </c>
       <c r="E6" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6">
-        <v>120</v>
+        <v>25</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="G6" t="s">
-        <v>36</v>
-      </c>
-      <c r="H6" t="s">
-        <v>25</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="K6" t="s">
-        <v>30</v>
-      </c>
-      <c r="L6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7" t="s">
         <v>16</v>
       </c>
-      <c r="C7" t="s">
-        <v>33</v>
+      <c r="C7">
+        <v>28201</v>
       </c>
       <c r="D7">
-        <v>28201</v>
+        <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
+        <v>26</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="G7" t="s">
-        <v>36</v>
-      </c>
-      <c r="H7" t="s">
-        <v>26</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="K7" t="s">
-        <v>41</v>
-      </c>
-      <c r="L7">
-        <v>1</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -905,7 +768,7 @@
         <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
         <v>15</v>
@@ -928,7 +791,7 @@
         <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -939,13 +802,13 @@
         <v>-1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
         <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -962,7 +825,7 @@
         <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>